<commit_message>
Put the object scripts into Verb { } Groups
</commit_message>
<xml_diff>
--- a/Release/ManiacMansion.xlsx
+++ b/Release/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="22320" windowHeight="9468" tabRatio="702" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="14136" windowHeight="8304" tabRatio="702" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="860">
   <si>
     <t>Purpose</t>
   </si>
@@ -2349,9 +2349,6 @@
     <t>Glass Chandelier</t>
   </si>
   <si>
-    <t>08 = Is Playing</t>
-  </si>
-  <si>
     <t>Loose Brick</t>
   </si>
   <si>
@@ -2608,6 +2605,18 @@
   </si>
   <si>
     <t>Room 36 Entered (Storage room next to Pool)</t>
+  </si>
+  <si>
+    <t>08 = In Player</t>
+  </si>
+  <si>
+    <t>08 = Has Tape</t>
+  </si>
+  <si>
+    <t>02 = Still  Alive</t>
+  </si>
+  <si>
+    <t>08 = In Microwave</t>
   </si>
 </sst>
 </file>
@@ -2939,7 +2948,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3185,7 +3194,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3193,7 +3202,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
   </sheetData>
@@ -3217,15 +3226,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>779</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B2" s="3">
         <v>4</v>
@@ -3233,7 +3242,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
@@ -3241,7 +3250,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B4" s="3">
         <v>6</v>
@@ -3249,7 +3258,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B5" s="3">
         <v>7</v>
@@ -3260,15 +3269,15 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -3286,7 +3295,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -3295,7 +3304,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
@@ -3304,7 +3313,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B13" s="3">
         <v>4</v>
@@ -3313,7 +3322,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
@@ -3322,7 +3331,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B15" s="3">
         <v>6</v>
@@ -3331,7 +3340,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B16" s="3">
         <v>7</v>
@@ -3340,7 +3349,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B17" s="3">
         <v>8</v>
@@ -3349,7 +3358,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B18" s="3">
         <v>9</v>
@@ -3358,55 +3367,55 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C24" s="3"/>
     </row>
@@ -4182,8 +4191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFC157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4275,7 +4284,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -4286,7 +4295,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -4418,7 +4427,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -4835,7 +4844,7 @@
         <v>18</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -21643,7 +21652,7 @@
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -21668,10 +21677,10 @@
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E95" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -21737,7 +21746,7 @@
         <v>18</v>
       </c>
       <c r="C101" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
@@ -22107,7 +22116,7 @@
         <v>18</v>
       </c>
       <c r="C133" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -22340,10 +22349,10 @@
         <v>323</v>
       </c>
       <c r="D152" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F152" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -22421,8 +22430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22558,7 +22567,7 @@
         <v>590</v>
       </c>
       <c r="E7" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F7" t="s">
         <v>591</v>
@@ -22671,7 +22680,7 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -22699,7 +22708,7 @@
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E16" t="s">
         <v>259</v>
@@ -22892,13 +22901,13 @@
         <v>48</v>
       </c>
       <c r="C36" t="s">
+        <v>843</v>
+      </c>
+      <c r="E36" t="s">
         <v>844</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>845</v>
-      </c>
-      <c r="F36" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -22909,13 +22918,13 @@
         <v>170</v>
       </c>
       <c r="D37" t="s">
+        <v>827</v>
+      </c>
+      <c r="E37" t="s">
         <v>828</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>829</v>
-      </c>
-      <c r="F37" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -22946,7 +22955,7 @@
         <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="E39" t="s">
         <v>217</v>
@@ -23395,7 +23404,7 @@
         <v>86</v>
       </c>
       <c r="C71" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
@@ -23411,13 +23420,13 @@
         <v>89</v>
       </c>
       <c r="C73" t="s">
+        <v>840</v>
+      </c>
+      <c r="E73" t="s">
+        <v>839</v>
+      </c>
+      <c r="F73" t="s">
         <v>841</v>
-      </c>
-      <c r="E73" t="s">
-        <v>840</v>
-      </c>
-      <c r="F73" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
@@ -23528,7 +23537,7 @@
         <v>101</v>
       </c>
       <c r="C85" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E85" t="s">
         <v>217</v>
@@ -23649,7 +23658,7 @@
         <v>109</v>
       </c>
       <c r="C93" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E93" t="s">
         <v>217</v>
@@ -23687,7 +23696,7 @@
         <v>113</v>
       </c>
       <c r="C97" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="E97" t="s">
         <v>217</v>
@@ -23698,7 +23707,7 @@
         <v>114</v>
       </c>
       <c r="C98" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E98" t="s">
         <v>217</v>
@@ -23707,12 +23716,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>116</v>
       </c>
       <c r="C99" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E99" t="s">
         <v>217</v>
@@ -23726,7 +23735,7 @@
         <v>117</v>
       </c>
       <c r="C100" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E100" t="s">
         <v>259</v>
@@ -23740,7 +23749,7 @@
         <v>118</v>
       </c>
       <c r="C101" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E101" t="s">
         <v>259</v>
@@ -23754,7 +23763,7 @@
         <v>119</v>
       </c>
       <c r="C102" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E102" t="s">
         <v>259</v>
@@ -23768,7 +23777,7 @@
         <v>120</v>
       </c>
       <c r="C103" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E103" t="s">
         <v>259</v>
@@ -23830,7 +23839,7 @@
         <v>128</v>
       </c>
       <c r="C107" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E107" t="s">
         <v>217</v>
@@ -23915,7 +23924,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -23995,7 +24004,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -24011,7 +24020,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -24043,7 +24052,7 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -24059,7 +24068,7 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -24147,7 +24156,7 @@
         <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -24187,7 +24196,7 @@
         <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -24226,8 +24235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H439"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A405" workbookViewId="0">
+      <selection activeCell="C405" sqref="C405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24341,9 +24350,6 @@
       <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="D7" t="s">
-        <v>766</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -24381,7 +24387,7 @@
         <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -24405,6 +24411,12 @@
       <c r="C12" t="s">
         <v>37</v>
       </c>
+      <c r="D12" t="s">
+        <v>766</v>
+      </c>
+      <c r="E12" t="s">
+        <v>733</v>
+      </c>
       <c r="G12" t="s">
         <v>68</v>
       </c>
@@ -24723,6 +24735,9 @@
       <c r="C39" t="s">
         <v>379</v>
       </c>
+      <c r="D39" t="s">
+        <v>856</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
@@ -24749,7 +24764,7 @@
         <v>380</v>
       </c>
       <c r="D41" t="s">
-        <v>770</v>
+        <v>857</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -24901,7 +24916,7 @@
         <v>446</v>
       </c>
       <c r="C54" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -25023,7 +25038,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>6</v>
       </c>
@@ -25037,7 +25052,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>6</v>
       </c>
@@ -25048,7 +25063,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>6</v>
       </c>
@@ -25062,7 +25077,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>6</v>
       </c>
@@ -25073,7 +25088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>6</v>
       </c>
@@ -25087,7 +25102,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>6</v>
       </c>
@@ -25098,7 +25113,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>6</v>
       </c>
@@ -25109,7 +25124,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>6</v>
       </c>
@@ -25120,7 +25135,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>7</v>
       </c>
@@ -25134,7 +25149,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>7</v>
       </c>
@@ -25148,7 +25163,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>7</v>
       </c>
@@ -25159,7 +25174,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>7</v>
       </c>
@@ -25170,7 +25185,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>7</v>
       </c>
@@ -25181,7 +25196,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>7</v>
       </c>
@@ -25191,8 +25206,14 @@
       <c r="C78" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D78" t="s">
+        <v>858</v>
+      </c>
+      <c r="E78" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>7</v>
       </c>
@@ -25202,8 +25223,14 @@
       <c r="C79" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D79" t="s">
+        <v>858</v>
+      </c>
+      <c r="E79" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>7</v>
       </c>
@@ -26007,7 +26034,7 @@
         <v>654</v>
       </c>
       <c r="D151" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
@@ -26337,7 +26364,7 @@
         <v>158</v>
       </c>
       <c r="C181" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D181" t="s">
         <v>754</v>
@@ -26362,7 +26389,10 @@
         <v>231</v>
       </c>
       <c r="C183" t="s">
-        <v>460</v>
+        <v>457</v>
+      </c>
+      <c r="D183" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
@@ -27372,7 +27402,7 @@
         <v>426</v>
       </c>
       <c r="D274" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.3">
@@ -27441,7 +27471,7 @@
         <v>426</v>
       </c>
       <c r="D280" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.3">
@@ -27455,7 +27485,7 @@
         <v>429</v>
       </c>
       <c r="D281" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.3">
@@ -27466,7 +27496,7 @@
         <v>239</v>
       </c>
       <c r="C282" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.3">
@@ -28769,7 +28799,7 @@
         <v>546</v>
       </c>
       <c r="D398" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.3">
@@ -28807,7 +28837,7 @@
         <v>287</v>
       </c>
       <c r="C402" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="403" spans="1:8" x14ac:dyDescent="0.3">
@@ -28817,7 +28847,7 @@
       <c r="B403">
         <v>288</v>
       </c>
-      <c r="C403">
+      <c r="C403" s="3">
         <v>0</v>
       </c>
     </row>
@@ -28828,8 +28858,8 @@
       <c r="B404">
         <v>289</v>
       </c>
-      <c r="C404" t="s">
-        <v>826</v>
+      <c r="C404" s="3" t="s">
+        <v>825</v>
       </c>
     </row>
     <row r="405" spans="1:8" x14ac:dyDescent="0.3">
@@ -28839,7 +28869,7 @@
       <c r="B405">
         <v>422</v>
       </c>
-      <c r="C405">
+      <c r="C405" s="3">
         <v>1</v>
       </c>
     </row>
@@ -28850,7 +28880,7 @@
       <c r="B406">
         <v>423</v>
       </c>
-      <c r="C406">
+      <c r="C406" s="3">
         <v>3</v>
       </c>
     </row>
@@ -28861,7 +28891,7 @@
       <c r="B407">
         <v>424</v>
       </c>
-      <c r="C407">
+      <c r="C407" s="3">
         <v>4</v>
       </c>
     </row>
@@ -28872,7 +28902,7 @@
       <c r="B408">
         <v>425</v>
       </c>
-      <c r="C408">
+      <c r="C408" s="3">
         <v>5</v>
       </c>
     </row>
@@ -28883,7 +28913,7 @@
       <c r="B409">
         <v>426</v>
       </c>
-      <c r="C409">
+      <c r="C409" s="3">
         <v>6</v>
       </c>
     </row>
@@ -28894,7 +28924,7 @@
       <c r="B410">
         <v>427</v>
       </c>
-      <c r="C410">
+      <c r="C410" s="3">
         <v>6</v>
       </c>
     </row>
@@ -28905,7 +28935,7 @@
       <c r="B411">
         <v>428</v>
       </c>
-      <c r="C411">
+      <c r="C411" s="3">
         <v>7</v>
       </c>
     </row>
@@ -28916,7 +28946,7 @@
       <c r="B412">
         <v>429</v>
       </c>
-      <c r="C412">
+      <c r="C412" s="3">
         <v>8</v>
       </c>
     </row>
@@ -28927,7 +28957,7 @@
       <c r="B413">
         <v>430</v>
       </c>
-      <c r="C413">
+      <c r="C413" s="3">
         <v>9</v>
       </c>
     </row>
@@ -29214,6 +29244,7 @@
     <sortCondition ref="B2:B439"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -29324,7 +29355,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29334,16 +29365,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -29351,13 +29382,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C2" t="s">
+        <v>809</v>
+      </c>
+      <c r="D2" t="s">
         <v>810</v>
-      </c>
-      <c r="D2" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -29365,10 +29396,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
   </sheetData>
@@ -29382,7 +29413,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add blocks for some beginOverride opcodes
</commit_message>
<xml_diff>
--- a/Release/ManiacMansion.xlsx
+++ b/Release/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="14136" windowHeight="8304" tabRatio="702" activeTab="3"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="20340" windowHeight="12960" tabRatio="702" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="869">
   <si>
     <t>Purpose</t>
   </si>
@@ -2568,21 +2568,9 @@
     <t>Nurse Edna: Out of room</t>
   </si>
   <si>
-    <t>Pin Entry Correct</t>
-  </si>
-  <si>
-    <t>0 = Yes</t>
-  </si>
-  <si>
-    <t>1 = No</t>
-  </si>
-  <si>
     <t>Dr. Fred / Nurse Edna Trigger Enabled</t>
   </si>
   <si>
-    <t>Keypad Input Complete</t>
-  </si>
-  <si>
     <t>08 = Fixed</t>
   </si>
   <si>
@@ -2617,6 +2605,45 @@
   </si>
   <si>
     <t>08 = In Microwave</t>
+  </si>
+  <si>
+    <t>Keypad Input Open</t>
+  </si>
+  <si>
+    <t>Pin Entry Wrong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02 = </t>
+  </si>
+  <si>
+    <t>script-48</t>
+  </si>
+  <si>
+    <t>Script does not stop</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>roomobj-7-60.Give</t>
+  </si>
+  <si>
+    <t>Green Tentacle Heard tape playing</t>
+  </si>
+  <si>
+    <t>script-102</t>
+  </si>
+  <si>
+    <t>08 = Hidden</t>
+  </si>
+  <si>
+    <t>08 = Lights On</t>
+  </si>
+  <si>
+    <t>Var 112 = 0 If Kid in Room</t>
+  </si>
+  <si>
+    <t>Loops until actor moves from gargoyle</t>
   </si>
 </sst>
 </file>
@@ -2948,7 +2975,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3430,7 +3457,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4191,20 +4218,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFC157"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="F145" sqref="F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="63.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -4220,8 +4247,11 @@
       <c r="E1" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4232,7 +4262,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4243,7 +4273,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4254,7 +4284,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4265,7 +4295,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4276,7 +4306,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4287,7 +4317,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4298,7 +4328,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4309,7 +4339,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4320,7 +4350,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4331,7 +4361,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4342,7 +4372,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4353,7 +4383,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4364,7 +4394,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4375,7 +4405,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4769,6 +4799,12 @@
       <c r="C49" t="s">
         <v>180</v>
       </c>
+      <c r="D49" t="s">
+        <v>862</v>
+      </c>
+      <c r="F49" t="s">
+        <v>860</v>
+      </c>
     </row>
     <row r="50" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A50">
@@ -4779,6 +4815,12 @@
       </c>
       <c r="C50" t="s">
         <v>201</v>
+      </c>
+      <c r="D50" t="s">
+        <v>859</v>
+      </c>
+      <c r="F50" t="s">
+        <v>860</v>
       </c>
     </row>
     <row r="51" spans="1:16383" x14ac:dyDescent="0.3">
@@ -21652,7 +21694,7 @@
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -21677,10 +21719,10 @@
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="E95" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -21873,7 +21915,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -21884,7 +21926,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -21898,7 +21940,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -21912,7 +21954,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -21926,7 +21968,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -21937,7 +21979,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -21948,7 +21990,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -21959,7 +22001,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -21970,7 +22012,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -21981,7 +22023,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -21992,7 +22034,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -22003,7 +22045,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -22014,7 +22056,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -22024,8 +22066,11 @@
       <c r="C125" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F125" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -22036,7 +22081,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -22050,7 +22095,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -22061,7 +22106,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -22072,7 +22117,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -22083,7 +22128,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -22097,7 +22142,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -22108,7 +22153,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -22119,7 +22164,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -22132,8 +22177,11 @@
       <c r="E134" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F134" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -22144,7 +22192,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -22155,7 +22203,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -22166,7 +22214,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -22177,7 +22225,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -22188,7 +22236,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -22199,7 +22247,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -22210,7 +22258,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -22224,7 +22272,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -22235,7 +22283,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -22259,6 +22307,9 @@
       <c r="C145" t="s">
         <v>488</v>
       </c>
+      <c r="F145" t="s">
+        <v>868</v>
+      </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
@@ -22349,10 +22400,10 @@
         <v>323</v>
       </c>
       <c r="D152" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="F152" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -22428,10 +22479,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22901,13 +22952,13 @@
         <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>843</v>
+        <v>857</v>
       </c>
       <c r="E36" t="s">
-        <v>844</v>
+        <v>217</v>
       </c>
       <c r="F36" t="s">
-        <v>845</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -22955,7 +23006,7 @@
         <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>847</v>
+        <v>856</v>
       </c>
       <c r="E39" t="s">
         <v>217</v>
@@ -23696,7 +23747,7 @@
         <v>113</v>
       </c>
       <c r="C97" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="E97" t="s">
         <v>217</v>
@@ -23707,7 +23758,7 @@
         <v>114</v>
       </c>
       <c r="C98" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="E98" t="s">
         <v>217</v>
@@ -23887,6 +23938,23 @@
       </c>
       <c r="C111" t="s">
         <v>559</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>138</v>
+      </c>
+      <c r="C112" t="s">
+        <v>863</v>
+      </c>
+      <c r="D112" t="s">
+        <v>864</v>
+      </c>
+      <c r="E112" t="s">
+        <v>217</v>
+      </c>
+      <c r="F112" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -23903,7 +23971,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24235,8 +24303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H439"/>
   <sheetViews>
-    <sheetView topLeftCell="A405" workbookViewId="0">
-      <selection activeCell="C405" sqref="C405"/>
+    <sheetView topLeftCell="A325" workbookViewId="0">
+      <selection activeCell="E357" sqref="E357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24736,7 +24804,7 @@
         <v>379</v>
       </c>
       <c r="D39" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -24764,7 +24832,7 @@
         <v>380</v>
       </c>
       <c r="D41" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -25207,10 +25275,10 @@
         <v>29</v>
       </c>
       <c r="D78" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="E78" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -25224,10 +25292,10 @@
         <v>411</v>
       </c>
       <c r="D79" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="E79" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -26034,7 +26102,7 @@
         <v>654</v>
       </c>
       <c r="D151" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
@@ -26852,7 +26920,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>19</v>
       </c>
@@ -26863,7 +26931,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>19</v>
       </c>
@@ -26874,7 +26942,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>19</v>
       </c>
@@ -26885,7 +26953,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>19</v>
       </c>
@@ -26896,7 +26964,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>20</v>
       </c>
@@ -26906,8 +26974,11 @@
       <c r="C229" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D229" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>20</v>
       </c>
@@ -26918,7 +26989,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>20</v>
       </c>
@@ -26929,7 +27000,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>20</v>
       </c>
@@ -26940,7 +27011,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>20</v>
       </c>
@@ -26951,7 +27022,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>20</v>
       </c>
@@ -26961,8 +27032,11 @@
       <c r="C234" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D234" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>20</v>
       </c>
@@ -26973,7 +27047,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>20</v>
       </c>
@@ -26984,7 +27058,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>20</v>
       </c>
@@ -26995,7 +27069,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>20</v>
       </c>
@@ -27006,7 +27080,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>20</v>
       </c>
@@ -27017,7 +27091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>20</v>
       </c>
@@ -27747,7 +27821,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>26</v>
       </c>
@@ -27758,7 +27832,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>26</v>
       </c>
@@ -27769,7 +27843,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>26</v>
       </c>
@@ -27780,7 +27854,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>26</v>
       </c>
@@ -27791,7 +27865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>26</v>
       </c>
@@ -27802,7 +27876,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>27</v>
       </c>
@@ -27813,7 +27887,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>27</v>
       </c>
@@ -27823,8 +27897,11 @@
       <c r="C311" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D311" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>27</v>
       </c>
@@ -27835,7 +27912,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>27</v>
       </c>
@@ -27846,7 +27923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>27</v>
       </c>
@@ -27856,8 +27933,11 @@
       <c r="C314" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D314" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>27</v>
       </c>
@@ -27868,7 +27948,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>27</v>
       </c>
@@ -27879,7 +27959,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>27</v>
       </c>
@@ -27890,7 +27970,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>27</v>
       </c>
@@ -27901,7 +27981,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>27</v>
       </c>
@@ -27912,7 +27992,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>27</v>
       </c>
@@ -28278,7 +28358,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>33</v>
       </c>
@@ -28291,8 +28371,11 @@
       <c r="D353" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E353" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>33</v>
       </c>
@@ -28305,8 +28388,11 @@
       <c r="D354" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E354" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>33</v>
       </c>
@@ -28319,8 +28405,11 @@
       <c r="D355" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E355" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>33</v>
       </c>
@@ -28333,8 +28422,11 @@
       <c r="D356" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E356" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>33</v>
       </c>
@@ -28347,8 +28439,11 @@
       <c r="D357" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E357" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>33</v>
       </c>
@@ -28359,7 +28454,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>34</v>
       </c>
@@ -28370,7 +28465,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>34</v>
       </c>
@@ -28381,7 +28476,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>34</v>
       </c>
@@ -28392,7 +28487,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>34</v>
       </c>
@@ -28403,7 +28498,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>35</v>
       </c>
@@ -28414,7 +28509,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>35</v>
       </c>
@@ -28425,7 +28520,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>36</v>
       </c>
@@ -28436,7 +28531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>36</v>
       </c>
@@ -28447,7 +28542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>36</v>
       </c>
@@ -28458,7 +28553,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>36</v>
       </c>
@@ -29399,7 +29494,7 @@
         <v>807</v>
       </c>
       <c r="C3" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
     </row>
   </sheetData>
@@ -29413,7 +29508,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add more blocks for beginOverride opcodes
</commit_message>
<xml_diff>
--- a/Release/ManiacMansion.xlsx
+++ b/Release/ManiacMansion.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="869">
   <si>
     <t>Purpose</t>
   </si>
@@ -4219,7 +4219,7 @@
   <dimension ref="A1:XFC157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="F145" sqref="F145"/>
+      <selection activeCell="F155" sqref="F155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22427,6 +22427,9 @@
       <c r="C154" t="s">
         <v>325</v>
       </c>
+      <c r="F154" t="s">
+        <v>860</v>
+      </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155">
@@ -22482,7 +22485,7 @@
   <dimension ref="A1:I112"/>
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Put the Demo object scripts into Verb { } Groups Change the Scripts into { } Groups
</commit_message>
<xml_diff>
--- a/Release/ManiacMansion.xlsx
+++ b/Release/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="20340" windowHeight="12960" tabRatio="702" activeTab="2"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="20340" windowHeight="12960" tabRatio="702" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -4218,8 +4218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFC157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="F155" sqref="F155"/>
+    <sheetView topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22484,8 +22484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29510,8 +29510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Name some variables Alignment of comments
</commit_message>
<xml_diff>
--- a/Release/ManiacMansion.xlsx
+++ b/Release/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="20340" windowHeight="12960" tabRatio="702" activeTab="3"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="14172" windowHeight="7632" tabRatio="702" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="880">
   <si>
     <t>Purpose</t>
   </si>
@@ -1839,9 +1839,6 @@
     <t>Door: Kitchen</t>
   </si>
   <si>
-    <t>Window Break</t>
-  </si>
-  <si>
     <t>Cassette: Play, Break Windows/Free Key</t>
   </si>
   <si>
@@ -2529,9 +2526,6 @@
     <t>11 = #</t>
   </si>
   <si>
-    <t>08 = in mailbox</t>
-  </si>
-  <si>
     <t>Cutscene: 3 Guys Who Pub Anything: Receive Mail Trigger</t>
   </si>
   <si>
@@ -2647,6 +2641,42 @@
   </si>
   <si>
     <t>04 = Broken</t>
+  </si>
+  <si>
+    <t>Coin</t>
+  </si>
+  <si>
+    <t>Shower On</t>
+  </si>
+  <si>
+    <t>08 = in Mailbox</t>
+  </si>
+  <si>
+    <t>Output Variable</t>
+  </si>
+  <si>
+    <t>Var 92: 1 - Flashlight. 2 - Light On</t>
+  </si>
+  <si>
+    <t>Ted: Bath Curtain Moving</t>
+  </si>
+  <si>
+    <t>Window Crack</t>
+  </si>
+  <si>
+    <t>Window 1</t>
+  </si>
+  <si>
+    <t>Window 2</t>
+  </si>
+  <si>
+    <t>Hunk-O-Matic Down</t>
+  </si>
+  <si>
+    <t>Hunk-O-Matic Up</t>
+  </si>
+  <si>
+    <t>Dial Tone</t>
   </si>
 </sst>
 </file>
@@ -3224,7 +3254,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3232,7 +3262,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
   </sheetData>
@@ -3256,15 +3286,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>778</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B2" s="3">
         <v>4</v>
@@ -3272,7 +3302,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
@@ -3280,7 +3310,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B4" s="3">
         <v>6</v>
@@ -3288,7 +3318,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B5" s="3">
         <v>7</v>
@@ -3299,15 +3329,15 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -3325,7 +3355,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -3334,7 +3364,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
@@ -3343,7 +3373,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B13" s="3">
         <v>4</v>
@@ -3352,7 +3382,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
@@ -3361,7 +3391,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B15" s="3">
         <v>6</v>
@@ -3370,7 +3400,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B16" s="3">
         <v>7</v>
@@ -3379,7 +3409,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B17" s="3">
         <v>8</v>
@@ -3388,7 +3418,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B18" s="3">
         <v>9</v>
@@ -3397,55 +3427,55 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C24" s="3"/>
     </row>
@@ -3894,7 +3924,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -4020,7 +4050,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
@@ -4219,10 +4249,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFC157"/>
+  <dimension ref="A1:XFD157"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4231,10 +4261,11 @@
     <col min="3" max="3" width="63.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" customWidth="1"/>
+    <col min="7" max="7" width="32.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -4251,10 +4282,13 @@
         <v>213</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>871</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4265,7 +4299,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4273,10 +4307,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4287,7 +4321,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4298,7 +4332,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4309,7 +4343,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4317,10 +4351,10 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4328,10 +4362,10 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4342,7 +4376,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4353,7 +4387,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4364,7 +4398,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4375,7 +4409,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4386,7 +4420,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4397,7 +4431,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4408,7 +4442,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4416,7 +4450,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -4460,7 +4494,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -4609,7 +4643,7 @@
         <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D33" t="s">
         <v>83</v>
@@ -4634,7 +4668,7 @@
         <v>18</v>
       </c>
       <c r="C35" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D35" t="s">
         <v>87</v>
@@ -4703,7 +4737,7 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -4778,7 +4812,7 @@
         <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -4792,7 +4826,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="49" spans="1:16383" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4803,13 +4837,13 @@
         <v>180</v>
       </c>
       <c r="D49" t="s">
-        <v>862</v>
-      </c>
-      <c r="F49" t="s">
         <v>860</v>
       </c>
-    </row>
-    <row r="50" spans="1:16383" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4820,13 +4854,13 @@
         <v>201</v>
       </c>
       <c r="D50" t="s">
-        <v>859</v>
-      </c>
-      <c r="F50" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16383" x14ac:dyDescent="0.3">
+        <v>857</v>
+      </c>
+      <c r="G50" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4836,8 +4870,11 @@
       <c r="C51" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="52" spans="1:16383" x14ac:dyDescent="0.3">
+      <c r="F51" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4848,7 +4885,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="53" spans="1:16383" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4859,7 +4896,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="54" spans="1:16383" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4870,7 +4907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:16383" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4881,7 +4918,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="56" spans="1:16383" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -4889,7 +4926,7 @@
         <v>18</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -21271,8 +21308,9 @@
       <c r="XFA56" s="2"/>
       <c r="XFB56" s="2"/>
       <c r="XFC56" s="2"/>
-    </row>
-    <row r="57" spans="1:16383" x14ac:dyDescent="0.3">
+      <c r="XFD56" s="2"/>
+    </row>
+    <row r="57" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -21280,13 +21318,13 @@
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E57" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="58" spans="1:16383" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -21300,7 +21338,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="59" spans="1:16383" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -21314,7 +21352,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:16383" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -21325,7 +21363,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="61" spans="1:16383" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -21336,7 +21374,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="62" spans="1:16383" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -21347,7 +21385,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="63" spans="1:16383" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -21358,7 +21396,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="64" spans="1:16383" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -21457,7 +21495,7 @@
         <v>18</v>
       </c>
       <c r="C72" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -21479,7 +21517,7 @@
         <v>18</v>
       </c>
       <c r="C74" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -21556,7 +21594,7 @@
         <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -21567,7 +21605,7 @@
         <v>18</v>
       </c>
       <c r="C82" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E82" t="s">
         <v>250</v>
@@ -21650,7 +21688,7 @@
         <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -21661,7 +21699,7 @@
         <v>18</v>
       </c>
       <c r="C90" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -21697,7 +21735,7 @@
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -21722,10 +21760,10 @@
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="E95" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -21791,7 +21829,7 @@
         <v>18</v>
       </c>
       <c r="C101" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
@@ -21915,10 +21953,10 @@
         <v>18</v>
       </c>
       <c r="C112" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -21929,7 +21967,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -21943,7 +21981,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -21957,7 +21995,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -21971,7 +22009,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -21982,7 +22020,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -21993,7 +22031,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -22004,7 +22042,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -22015,7 +22053,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -22026,7 +22064,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -22037,7 +22075,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -22048,7 +22086,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -22059,7 +22097,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -22069,11 +22107,11 @@
       <c r="C125" t="s">
         <v>299</v>
       </c>
-      <c r="F125" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G125" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -22084,7 +22122,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -22098,7 +22136,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -22109,7 +22147,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -22120,7 +22158,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -22131,7 +22169,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -22145,7 +22183,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -22156,7 +22194,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -22164,10 +22202,10 @@
         <v>18</v>
       </c>
       <c r="C133" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -22180,11 +22218,11 @@
       <c r="E134" t="s">
         <v>594</v>
       </c>
-      <c r="F134" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G134" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -22195,7 +22233,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -22206,7 +22244,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -22217,7 +22255,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -22228,7 +22266,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -22239,7 +22277,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -22250,7 +22288,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -22261,7 +22299,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -22275,7 +22313,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -22286,7 +22324,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -22300,7 +22338,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
@@ -22310,11 +22348,11 @@
       <c r="C145" t="s">
         <v>488</v>
       </c>
-      <c r="F145" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G145" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
@@ -22325,7 +22363,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>146</v>
       </c>
@@ -22339,7 +22377,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>147</v>
       </c>
@@ -22353,7 +22391,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>148</v>
       </c>
@@ -22367,7 +22405,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>149</v>
       </c>
@@ -22378,7 +22416,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
@@ -22392,7 +22430,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>151</v>
       </c>
@@ -22403,13 +22441,13 @@
         <v>323</v>
       </c>
       <c r="D152" t="s">
-        <v>848</v>
-      </c>
-      <c r="F152" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+        <v>846</v>
+      </c>
+      <c r="G152" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>154</v>
       </c>
@@ -22420,7 +22458,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>155</v>
       </c>
@@ -22430,11 +22468,11 @@
       <c r="C154" t="s">
         <v>325</v>
       </c>
-      <c r="F154" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G154" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>156</v>
       </c>
@@ -22445,7 +22483,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>157</v>
       </c>
@@ -22453,10 +22491,10 @@
         <v>18</v>
       </c>
       <c r="C156" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>158</v>
       </c>
@@ -22464,7 +22502,7 @@
         <v>18</v>
       </c>
       <c r="C157" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D157" t="s">
         <v>326</v>
@@ -22485,10 +22523,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I112"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22536,10 +22574,10 @@
         <v>218</v>
       </c>
       <c r="G2" t="s">
+        <v>734</v>
+      </c>
+      <c r="H2" t="s">
         <v>735</v>
-      </c>
-      <c r="H2" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -22610,10 +22648,10 @@
         <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F6" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -22624,7 +22662,7 @@
         <v>590</v>
       </c>
       <c r="E7" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F7" t="s">
         <v>591</v>
@@ -22649,137 +22687,137 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
+        <v>603</v>
+      </c>
+      <c r="E9" t="s">
         <v>604</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>605</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>606</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>607</v>
-      </c>
-      <c r="H9" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>236</v>
+        <v>873</v>
       </c>
       <c r="E10" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F10" t="s">
-        <v>631</v>
-      </c>
-      <c r="G10" t="s">
-        <v>240</v>
-      </c>
-      <c r="H10" t="s">
-        <v>431</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="E11" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
       <c r="F11" t="s">
-        <v>243</v>
+        <v>630</v>
+      </c>
+      <c r="G11" t="s">
+        <v>240</v>
+      </c>
+      <c r="H11" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>238</v>
+        <v>260</v>
       </c>
       <c r="E12" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="F12" t="s">
-        <v>631</v>
-      </c>
-      <c r="G12" t="s">
-        <v>240</v>
-      </c>
-      <c r="H12" t="s">
-        <v>431</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>609</v>
+        <v>238</v>
       </c>
       <c r="E13" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="F13" t="s">
-        <v>218</v>
+        <v>630</v>
+      </c>
+      <c r="G13" t="s">
+        <v>240</v>
+      </c>
+      <c r="H13" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>824</v>
+        <v>608</v>
+      </c>
+      <c r="E14" t="s">
+        <v>217</v>
+      </c>
+      <c r="F14" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>245</v>
-      </c>
-      <c r="E15" t="s">
-        <v>229</v>
-      </c>
-      <c r="F15" t="s">
-        <v>631</v>
-      </c>
-      <c r="G15" t="s">
-        <v>240</v>
-      </c>
-      <c r="H15" t="s">
-        <v>431</v>
+        <v>823</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>806</v>
+        <v>245</v>
       </c>
       <c r="E16" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
       <c r="F16" t="s">
-        <v>243</v>
+        <v>630</v>
+      </c>
+      <c r="G16" t="s">
+        <v>240</v>
+      </c>
+      <c r="H16" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>805</v>
       </c>
       <c r="E17" t="s">
         <v>259</v>
@@ -22790,221 +22828,212 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>715</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>716</v>
+        <v>259</v>
       </c>
       <c r="F18" t="s">
-        <v>717</v>
-      </c>
-      <c r="G18" t="s">
-        <v>718</v>
-      </c>
-      <c r="H18" t="s">
-        <v>719</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>596</v>
+        <v>714</v>
       </c>
       <c r="E19" t="s">
-        <v>217</v>
+        <v>715</v>
       </c>
       <c r="F19" t="s">
-        <v>597</v>
+        <v>716</v>
       </c>
       <c r="G19" t="s">
-        <v>598</v>
+        <v>717</v>
+      </c>
+      <c r="H19" t="s">
+        <v>718</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>163</v>
+        <v>596</v>
+      </c>
+      <c r="E20" t="s">
+        <v>217</v>
+      </c>
+      <c r="F20" t="s">
+        <v>597</v>
+      </c>
+      <c r="G20" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>264</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>857</v>
-      </c>
-      <c r="E36" t="s">
-        <v>217</v>
-      </c>
-      <c r="F36" t="s">
-        <v>218</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>170</v>
-      </c>
-      <c r="D37" t="s">
-        <v>827</v>
+        <v>855</v>
       </c>
       <c r="E37" t="s">
-        <v>828</v>
+        <v>217</v>
       </c>
       <c r="F37" t="s">
-        <v>829</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="D38" t="s">
-        <v>611</v>
+        <v>826</v>
       </c>
       <c r="E38" t="s">
-        <v>121</v>
+        <v>827</v>
       </c>
       <c r="F38" t="s">
-        <v>124</v>
-      </c>
-      <c r="G38" t="s">
-        <v>123</v>
-      </c>
-      <c r="H38" t="s">
-        <v>122</v>
+        <v>828</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -23012,170 +23041,179 @@
         <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>856</v>
+        <v>120</v>
+      </c>
+      <c r="D39" t="s">
+        <v>610</v>
       </c>
       <c r="E39" t="s">
-        <v>217</v>
+        <v>121</v>
       </c>
       <c r="F39" t="s">
-        <v>218</v>
+        <v>124</v>
+      </c>
+      <c r="G39" t="s">
+        <v>123</v>
+      </c>
+      <c r="H39" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>54</v>
-      </c>
-      <c r="B40" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" t="s">
-        <v>82</v>
+        <v>854</v>
+      </c>
+      <c r="E40" t="s">
+        <v>217</v>
+      </c>
+      <c r="F40" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>701</v>
-      </c>
-      <c r="E41" t="s">
-        <v>217</v>
-      </c>
-      <c r="F41" t="s">
-        <v>218</v>
+        <v>81</v>
+      </c>
+      <c r="D41" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="E42" t="s">
-        <v>293</v>
+        <v>217</v>
       </c>
       <c r="F42" t="s">
-        <v>294</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>173</v>
+        <v>706</v>
       </c>
       <c r="E43" t="s">
-        <v>174</v>
+        <v>293</v>
       </c>
       <c r="F43" t="s">
-        <v>175</v>
-      </c>
-      <c r="G43" t="s">
-        <v>176</v>
-      </c>
-      <c r="H43" t="s">
-        <v>177</v>
-      </c>
-      <c r="I43" t="s">
-        <v>178</v>
+        <v>294</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C44" t="s">
-        <v>159</v>
+        <v>173</v>
+      </c>
+      <c r="E44" t="s">
+        <v>174</v>
+      </c>
+      <c r="F44" t="s">
+        <v>175</v>
+      </c>
+      <c r="G44" t="s">
+        <v>176</v>
+      </c>
+      <c r="H44" t="s">
+        <v>177</v>
+      </c>
+      <c r="I44" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
+        <v>60</v>
+      </c>
+      <c r="C47" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48">
         <v>61</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
         <v>62</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="1"/>
-      <c r="E48" t="s">
+      <c r="D49" s="1"/>
+      <c r="E49" t="s">
         <v>59</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>63</v>
-      </c>
-      <c r="C49" t="s">
-        <v>762</v>
-      </c>
-      <c r="E49" t="s">
-        <v>229</v>
-      </c>
-      <c r="F49" t="s">
-        <v>247</v>
-      </c>
-      <c r="G49" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="E50" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="F50" t="s">
-        <v>218</v>
+        <v>247</v>
+      </c>
+      <c r="G50" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C51" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E51" t="s">
         <v>217</v>
@@ -23186,356 +23224,356 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52" t="s">
-        <v>204</v>
+        <v>760</v>
       </c>
       <c r="E52" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F52" t="s">
-        <v>401</v>
-      </c>
-      <c r="G52" t="s">
-        <v>230</v>
-      </c>
-      <c r="H52" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C53" t="s">
-        <v>548</v>
+        <v>204</v>
+      </c>
+      <c r="E53" t="s">
+        <v>229</v>
+      </c>
+      <c r="F53" t="s">
+        <v>401</v>
+      </c>
+      <c r="G53" t="s">
+        <v>230</v>
+      </c>
+      <c r="H53" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>68</v>
-      </c>
-      <c r="B54" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
-      </c>
-      <c r="D54" t="s">
-        <v>22</v>
-      </c>
-      <c r="E54" t="s">
-        <v>217</v>
-      </c>
-      <c r="F54" t="s">
-        <v>27</v>
+        <v>548</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>739</v>
+        <v>25</v>
+      </c>
+      <c r="D55" t="s">
+        <v>22</v>
       </c>
       <c r="E55" t="s">
-        <v>740</v>
+        <v>217</v>
+      </c>
+      <c r="F55" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
       </c>
       <c r="C56" t="s">
+        <v>738</v>
+      </c>
+      <c r="E56" t="s">
         <v>739</v>
-      </c>
-      <c r="E56" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>743</v>
+        <v>738</v>
+      </c>
+      <c r="E57" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>64</v>
-      </c>
-      <c r="E59" t="s">
-        <v>65</v>
-      </c>
-      <c r="F59" t="s">
-        <v>256</v>
-      </c>
-      <c r="G59" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>714</v>
+        <v>64</v>
       </c>
       <c r="E60" t="s">
-        <v>218</v>
+        <v>65</v>
+      </c>
+      <c r="F60" t="s">
+        <v>256</v>
+      </c>
+      <c r="G60" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61" t="s">
-        <v>457</v>
+        <v>713</v>
       </c>
       <c r="E61" t="s">
-        <v>277</v>
+        <v>218</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C62" t="s">
-        <v>208</v>
+        <v>457</v>
       </c>
       <c r="E62" t="s">
-        <v>205</v>
-      </c>
-      <c r="F62" t="s">
-        <v>722</v>
-      </c>
-      <c r="G62" t="s">
-        <v>206</v>
-      </c>
-      <c r="H62" t="s">
-        <v>281</v>
-      </c>
-      <c r="I62" t="s">
-        <v>207</v>
+        <v>277</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C63" t="s">
-        <v>723</v>
+        <v>208</v>
       </c>
       <c r="E63" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F63" t="s">
-        <v>211</v>
+        <v>721</v>
+      </c>
+      <c r="G63" t="s">
+        <v>206</v>
+      </c>
+      <c r="H63" t="s">
+        <v>281</v>
+      </c>
+      <c r="I63" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
+        <v>78</v>
+      </c>
+      <c r="C64" t="s">
+        <v>722</v>
+      </c>
+      <c r="E64" t="s">
+        <v>210</v>
+      </c>
+      <c r="F64" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65">
         <v>79</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>327</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E65" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65">
+    <row r="66" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66">
         <v>80</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>329</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E66" t="s">
         <v>217</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F66" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <v>81</v>
-      </c>
-      <c r="B66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s">
-        <v>57</v>
-      </c>
-      <c r="E66" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>547</v>
+        <v>57</v>
       </c>
       <c r="E67" t="s">
-        <v>284</v>
-      </c>
-      <c r="F67" t="s">
-        <v>282</v>
-      </c>
-      <c r="G67" t="s">
-        <v>283</v>
-      </c>
-      <c r="H67" t="s">
-        <v>568</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C68" t="s">
-        <v>549</v>
+        <v>547</v>
+      </c>
+      <c r="E68" t="s">
+        <v>284</v>
+      </c>
+      <c r="F68" t="s">
+        <v>282</v>
+      </c>
+      <c r="G68" t="s">
+        <v>283</v>
+      </c>
+      <c r="H68" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C69" t="s">
-        <v>388</v>
-      </c>
-      <c r="E69" t="s">
-        <v>217</v>
-      </c>
-      <c r="F69" t="s">
-        <v>389</v>
+        <v>549</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C70" t="s">
-        <v>765</v>
+        <v>388</v>
       </c>
       <c r="E70" t="s">
         <v>217</v>
       </c>
       <c r="F70" t="s">
-        <v>218</v>
+        <v>389</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C71" t="s">
-        <v>813</v>
+        <v>764</v>
+      </c>
+      <c r="E71" t="s">
+        <v>217</v>
+      </c>
+      <c r="F71" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C72" t="s">
-        <v>750</v>
+        <v>812</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C73" t="s">
-        <v>840</v>
-      </c>
-      <c r="E73" t="s">
-        <v>839</v>
-      </c>
-      <c r="F73" t="s">
-        <v>841</v>
+        <v>749</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>90</v>
-      </c>
-      <c r="D74" t="s">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="C74" t="s">
+        <v>838</v>
+      </c>
+      <c r="E74" t="s">
+        <v>837</v>
+      </c>
+      <c r="F74" t="s">
+        <v>839</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>90</v>
       </c>
-      <c r="B75" t="s">
-        <v>7</v>
-      </c>
-      <c r="C75" t="s">
-        <v>102</v>
+      <c r="D75" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>91</v>
-      </c>
-      <c r="D76" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>91</v>
       </c>
-      <c r="B77" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" t="s">
-        <v>101</v>
-      </c>
       <c r="D77" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D78" t="s">
         <v>88</v>
@@ -23543,72 +23581,72 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>94</v>
+        <v>92</v>
+      </c>
+      <c r="B79" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
+        <v>103</v>
+      </c>
+      <c r="D79" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>96</v>
-      </c>
-      <c r="C80" t="s">
-        <v>216</v>
-      </c>
-      <c r="E80" t="s">
-        <v>217</v>
-      </c>
-      <c r="F80" t="s">
-        <v>218</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C81" t="s">
-        <v>105</v>
+        <v>216</v>
+      </c>
+      <c r="E81" t="s">
+        <v>217</v>
+      </c>
+      <c r="F81" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C83" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="C84" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>101</v>
-      </c>
-      <c r="C85" t="s">
-        <v>771</v>
-      </c>
-      <c r="E85" t="s">
-        <v>217</v>
-      </c>
-      <c r="F85" t="s">
-        <v>218</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C86" t="s">
-        <v>742</v>
+        <v>770</v>
       </c>
       <c r="E86" t="s">
         <v>217</v>
@@ -23619,166 +23657,166 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C87" t="s">
-        <v>706</v>
-      </c>
-      <c r="D87" t="s">
-        <v>74</v>
+        <v>741</v>
       </c>
       <c r="E87" t="s">
-        <v>75</v>
+        <v>217</v>
       </c>
       <c r="F87" t="s">
-        <v>703</v>
-      </c>
-      <c r="G87" t="s">
-        <v>702</v>
+        <v>218</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C88" t="s">
-        <v>752</v>
+        <v>705</v>
+      </c>
+      <c r="D88" t="s">
+        <v>74</v>
       </c>
       <c r="E88" t="s">
-        <v>217</v>
+        <v>75</v>
       </c>
       <c r="F88" t="s">
-        <v>218</v>
+        <v>702</v>
+      </c>
+      <c r="G88" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>105</v>
-      </c>
-      <c r="B89" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C89" t="s">
-        <v>128</v>
+        <v>751</v>
+      </c>
+      <c r="E89" t="s">
+        <v>217</v>
+      </c>
+      <c r="F89" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B90" t="s">
         <v>7</v>
       </c>
       <c r="C90" t="s">
-        <v>711</v>
-      </c>
-      <c r="E90" t="s">
-        <v>712</v>
-      </c>
-      <c r="F90" t="s">
-        <v>127</v>
-      </c>
-      <c r="G90" t="s">
-        <v>713</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="B91" t="s">
+        <v>7</v>
       </c>
       <c r="C91" t="s">
-        <v>759</v>
+        <v>710</v>
+      </c>
+      <c r="E91" t="s">
+        <v>711</v>
+      </c>
+      <c r="F91" t="s">
+        <v>127</v>
+      </c>
+      <c r="G91" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C92" t="s">
-        <v>306</v>
-      </c>
-      <c r="E92" t="s">
-        <v>302</v>
-      </c>
-      <c r="F92" t="s">
-        <v>303</v>
-      </c>
-      <c r="G92" t="s">
-        <v>304</v>
-      </c>
-      <c r="H92" t="s">
-        <v>305</v>
+        <v>758</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C93" t="s">
-        <v>842</v>
+        <v>306</v>
       </c>
       <c r="E93" t="s">
-        <v>217</v>
+        <v>302</v>
       </c>
       <c r="F93" t="s">
-        <v>389</v>
+        <v>303</v>
+      </c>
+      <c r="G93" t="s">
+        <v>304</v>
+      </c>
+      <c r="H93" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C94" t="s">
-        <v>482</v>
+        <v>840</v>
       </c>
       <c r="E94" t="s">
         <v>217</v>
       </c>
       <c r="F94" t="s">
-        <v>218</v>
+        <v>389</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="C95" t="s">
+        <v>482</v>
+      </c>
+      <c r="E95" t="s">
+        <v>217</v>
+      </c>
+      <c r="F95" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>113</v>
-      </c>
-      <c r="C97" t="s">
-        <v>851</v>
-      </c>
-      <c r="E97" t="s">
-        <v>217</v>
+        <v>112</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C98" t="s">
-        <v>843</v>
+        <v>849</v>
       </c>
       <c r="E98" t="s">
         <v>217</v>
       </c>
-      <c r="F98" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C99" t="s">
-        <v>823</v>
+        <v>841</v>
       </c>
       <c r="E99" t="s">
         <v>217</v>
@@ -23787,26 +23825,26 @@
         <v>218</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C100" t="s">
-        <v>773</v>
+        <v>822</v>
       </c>
       <c r="E100" t="s">
-        <v>259</v>
+        <v>217</v>
       </c>
       <c r="F100" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C101" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E101" t="s">
         <v>259</v>
@@ -23817,10 +23855,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C102" t="s">
-        <v>812</v>
+        <v>772</v>
       </c>
       <c r="E102" t="s">
         <v>259</v>
@@ -23831,7 +23869,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C103" t="s">
         <v>811</v>
@@ -23845,121 +23883,135 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>122</v>
-      </c>
-      <c r="B104" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="C104" t="s">
-        <v>73</v>
-      </c>
-      <c r="D104" t="s">
-        <v>71</v>
+        <v>810</v>
       </c>
       <c r="E104" t="s">
-        <v>69</v>
+        <v>259</v>
       </c>
       <c r="F104" t="s">
-        <v>70</v>
+        <v>243</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="B105" t="s">
+        <v>6</v>
       </c>
       <c r="C105" t="s">
-        <v>595</v>
+        <v>73</v>
+      </c>
+      <c r="D105" t="s">
+        <v>71</v>
+      </c>
+      <c r="E105" t="s">
+        <v>69</v>
+      </c>
+      <c r="F105" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>127</v>
-      </c>
-      <c r="B106" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C106" t="s">
-        <v>20</v>
-      </c>
-      <c r="D106" t="s">
-        <v>22</v>
-      </c>
-      <c r="E106" t="s">
-        <v>21</v>
-      </c>
-      <c r="F106" t="s">
-        <v>26</v>
+        <v>595</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>128</v>
+        <v>127</v>
+      </c>
+      <c r="B107" t="s">
+        <v>7</v>
       </c>
       <c r="C107" t="s">
-        <v>803</v>
+        <v>20</v>
+      </c>
+      <c r="D107" t="s">
+        <v>22</v>
       </c>
       <c r="E107" t="s">
-        <v>217</v>
+        <v>21</v>
       </c>
       <c r="F107" t="s">
-        <v>218</v>
+        <v>26</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C108" t="s">
-        <v>751</v>
+        <v>802</v>
+      </c>
+      <c r="E108" t="s">
+        <v>217</v>
+      </c>
+      <c r="F108" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C109" t="s">
-        <v>753</v>
-      </c>
-      <c r="E109" t="s">
-        <v>217</v>
-      </c>
-      <c r="F109" t="s">
-        <v>218</v>
+        <v>750</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C110" t="s">
-        <v>589</v>
+        <v>752</v>
       </c>
       <c r="E110" t="s">
+        <v>217</v>
+      </c>
+      <c r="F110" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C111" t="s">
-        <v>559</v>
+        <v>589</v>
+      </c>
+      <c r="E111" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
+        <v>137</v>
+      </c>
+      <c r="C112" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113">
         <v>138</v>
       </c>
-      <c r="C112" t="s">
-        <v>863</v>
-      </c>
-      <c r="D112" t="s">
-        <v>864</v>
-      </c>
-      <c r="E112" t="s">
+      <c r="C113" t="s">
+        <v>861</v>
+      </c>
+      <c r="D113" t="s">
+        <v>862</v>
+      </c>
+      <c r="E113" t="s">
         <v>217</v>
       </c>
-      <c r="F112" t="s">
+      <c r="F113" t="s">
         <v>218</v>
       </c>
     </row>
@@ -23974,10 +24026,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23998,7 +24050,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -24027,34 +24079,34 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>365</v>
+        <v>868</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>709</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>564</v>
+        <v>708</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>564</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -24062,239 +24114,279 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>721</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>563</v>
+        <v>720</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>819</v>
+        <v>563</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>612</v>
+        <v>818</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>817</v>
+        <v>869</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>695</v>
+        <v>611</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>694</v>
+        <v>816</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>693</v>
+        <v>879</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>832</v>
+        <v>694</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>600</v>
+        <v>693</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>814</v>
+        <v>692</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>610</v>
+        <v>830</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>727</v>
+        <v>874</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>728</v>
+        <v>813</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>427</v>
+        <v>609</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>543</v>
+        <v>877</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>560</v>
+        <v>878</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>400</v>
+        <v>726</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>734</v>
+        <v>727</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>720</v>
+        <v>427</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>729</v>
+        <v>543</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>833</v>
+        <v>560</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>562</v>
+        <v>400</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>584</v>
+        <v>733</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>569</v>
+        <v>728</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>613</v>
+        <v>562</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>195</v>
+        <v>584</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>59</v>
+      </c>
+      <c r="B41" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>60</v>
+      </c>
+      <c r="B42" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>62</v>
+      </c>
+      <c r="B43" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
         <v>69</v>
       </c>
-      <c r="B39" t="s">
-        <v>726</v>
+      <c r="B44" t="s">
+        <v>725</v>
       </c>
     </row>
   </sheetData>
@@ -24309,8 +24401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H439"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24338,7 +24430,7 @@
         <v>383</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>51</v>
@@ -24355,7 +24447,7 @@
         <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -24369,7 +24461,7 @@
         <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -24394,10 +24486,10 @@
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="E5" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G5" t="s">
         <v>61</v>
@@ -24417,7 +24509,7 @@
         <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -24453,7 +24545,7 @@
         <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -24467,7 +24559,7 @@
         <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>830</v>
+        <v>870</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -24492,10 +24584,10 @@
         <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E12" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G12" t="s">
         <v>68</v>
@@ -24711,7 +24803,7 @@
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -24722,7 +24814,7 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -24744,7 +24836,7 @@
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -24755,7 +24847,7 @@
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -24780,7 +24872,7 @@
         <v>381</v>
       </c>
       <c r="D36" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -24791,7 +24883,7 @@
         <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>875</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -24802,7 +24894,7 @@
         <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>876</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -24816,7 +24908,7 @@
         <v>379</v>
       </c>
       <c r="D39" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -24830,7 +24922,7 @@
         <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -24844,7 +24936,7 @@
         <v>380</v>
       </c>
       <c r="D41" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -24880,7 +24972,7 @@
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -24894,7 +24986,7 @@
         <v>357</v>
       </c>
       <c r="D45" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -24930,7 +25022,7 @@
         <v>354</v>
       </c>
       <c r="D48" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -24996,7 +25088,7 @@
         <v>446</v>
       </c>
       <c r="C54" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -25010,7 +25102,7 @@
         <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -25027,7 +25119,7 @@
         <v>453</v>
       </c>
       <c r="E56" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -25129,7 +25221,7 @@
         <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -25151,10 +25243,10 @@
         <v>106</v>
       </c>
       <c r="C67" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D67" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -25179,7 +25271,7 @@
         <v>372</v>
       </c>
       <c r="D69" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -25212,7 +25304,7 @@
         <v>324</v>
       </c>
       <c r="C72" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -25226,7 +25318,7 @@
         <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -25240,7 +25332,7 @@
         <v>10</v>
       </c>
       <c r="D74" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -25287,10 +25379,10 @@
         <v>29</v>
       </c>
       <c r="D78" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="E78" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -25304,10 +25396,10 @@
         <v>411</v>
       </c>
       <c r="D79" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="E79" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -25332,7 +25424,7 @@
         <v>419</v>
       </c>
       <c r="D81" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -25500,7 +25592,7 @@
         <v>362</v>
       </c>
       <c r="D96" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -25808,7 +25900,7 @@
         <v>150</v>
       </c>
       <c r="C124" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -25819,7 +25911,7 @@
         <v>151</v>
       </c>
       <c r="C125" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -25830,7 +25922,7 @@
         <v>354</v>
       </c>
       <c r="C126" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -25841,7 +25933,7 @@
         <v>355</v>
       </c>
       <c r="C127" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
@@ -25979,7 +26071,7 @@
         <v>360</v>
       </c>
       <c r="C139" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
@@ -25990,7 +26082,7 @@
         <v>361</v>
       </c>
       <c r="C140" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
@@ -26012,7 +26104,7 @@
         <v>165</v>
       </c>
       <c r="C142" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
@@ -26023,7 +26115,7 @@
         <v>166</v>
       </c>
       <c r="C143" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
@@ -26034,7 +26126,7 @@
         <v>167</v>
       </c>
       <c r="C144" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
@@ -26045,7 +26137,7 @@
         <v>362</v>
       </c>
       <c r="C145" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
@@ -26056,7 +26148,7 @@
         <v>363</v>
       </c>
       <c r="C146" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
@@ -26067,7 +26159,7 @@
         <v>364</v>
       </c>
       <c r="C147" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
@@ -26078,7 +26170,7 @@
         <v>365</v>
       </c>
       <c r="C148" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
@@ -26089,7 +26181,7 @@
         <v>366</v>
       </c>
       <c r="C149" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
@@ -26111,10 +26203,10 @@
         <v>204</v>
       </c>
       <c r="C151" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D151" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
@@ -26125,7 +26217,7 @@
         <v>399</v>
       </c>
       <c r="C152" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
@@ -26147,7 +26239,7 @@
         <v>415</v>
       </c>
       <c r="C154" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
@@ -26444,10 +26536,10 @@
         <v>158</v>
       </c>
       <c r="C181" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D181" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
@@ -26472,7 +26564,7 @@
         <v>457</v>
       </c>
       <c r="D183" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
@@ -26538,7 +26630,7 @@
         <v>169</v>
       </c>
       <c r="C189" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
@@ -26549,7 +26641,7 @@
         <v>170</v>
       </c>
       <c r="C190" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
@@ -26560,7 +26652,7 @@
         <v>171</v>
       </c>
       <c r="C191" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
@@ -26571,7 +26663,7 @@
         <v>172</v>
       </c>
       <c r="C192" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -26582,7 +26674,7 @@
         <v>173</v>
       </c>
       <c r="C193" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
@@ -26593,7 +26685,7 @@
         <v>174</v>
       </c>
       <c r="C194" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
@@ -26604,7 +26696,7 @@
         <v>215</v>
       </c>
       <c r="C195" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -26615,7 +26707,7 @@
         <v>216</v>
       </c>
       <c r="C196" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
@@ -26626,7 +26718,7 @@
         <v>217</v>
       </c>
       <c r="C197" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
@@ -26637,7 +26729,7 @@
         <v>218</v>
       </c>
       <c r="C198" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
@@ -26648,7 +26740,7 @@
         <v>219</v>
       </c>
       <c r="C199" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
@@ -26659,7 +26751,7 @@
         <v>220</v>
       </c>
       <c r="C200" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
@@ -26736,7 +26828,7 @@
         <v>367</v>
       </c>
       <c r="C207" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
@@ -26747,7 +26839,7 @@
         <v>368</v>
       </c>
       <c r="C208" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
@@ -26758,7 +26850,7 @@
         <v>431</v>
       </c>
       <c r="C209" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
@@ -26769,7 +26861,7 @@
         <v>432</v>
       </c>
       <c r="C210" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
@@ -26780,7 +26872,7 @@
         <v>433</v>
       </c>
       <c r="C211" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
@@ -26791,7 +26883,7 @@
         <v>434</v>
       </c>
       <c r="C212" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
@@ -26802,7 +26894,7 @@
         <v>435</v>
       </c>
       <c r="C213" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
@@ -26813,7 +26905,7 @@
         <v>436</v>
       </c>
       <c r="C214" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
@@ -26838,10 +26930,10 @@
         <v>447</v>
       </c>
       <c r="D216" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E216" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
@@ -26987,7 +27079,7 @@
         <v>551</v>
       </c>
       <c r="D229" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
@@ -27045,7 +27137,7 @@
         <v>557</v>
       </c>
       <c r="D234" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
@@ -27243,7 +27335,7 @@
         <v>177</v>
       </c>
       <c r="C252" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
@@ -27254,7 +27346,7 @@
         <v>369</v>
       </c>
       <c r="C253" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
@@ -27265,7 +27357,7 @@
         <v>370</v>
       </c>
       <c r="C254" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
@@ -27276,7 +27368,7 @@
         <v>371</v>
       </c>
       <c r="C255" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
@@ -27298,7 +27390,7 @@
         <v>373</v>
       </c>
       <c r="C257" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
@@ -27309,7 +27401,7 @@
         <v>374</v>
       </c>
       <c r="C258" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
@@ -27320,7 +27412,7 @@
         <v>375</v>
       </c>
       <c r="C259" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
@@ -27331,7 +27423,7 @@
         <v>376</v>
       </c>
       <c r="C260" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
@@ -27342,7 +27434,7 @@
         <v>377</v>
       </c>
       <c r="C261" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
@@ -27353,7 +27445,7 @@
         <v>412</v>
       </c>
       <c r="C262" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
@@ -27375,7 +27467,7 @@
         <v>382</v>
       </c>
       <c r="C264" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
@@ -27386,7 +27478,7 @@
         <v>383</v>
       </c>
       <c r="C265" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
@@ -27408,7 +27500,7 @@
         <v>385</v>
       </c>
       <c r="C267" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.3">
@@ -27419,7 +27511,7 @@
         <v>413</v>
       </c>
       <c r="C268" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
@@ -27488,7 +27580,7 @@
         <v>426</v>
       </c>
       <c r="D274" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.3">
@@ -27557,7 +27649,7 @@
         <v>426</v>
       </c>
       <c r="D280" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.3">
@@ -27571,7 +27663,7 @@
         <v>429</v>
       </c>
       <c r="D281" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.3">
@@ -27582,7 +27674,7 @@
         <v>239</v>
       </c>
       <c r="C282" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.3">
@@ -27659,10 +27751,10 @@
         <v>77</v>
       </c>
       <c r="C289" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D289" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.3">
@@ -27673,7 +27765,7 @@
         <v>78</v>
       </c>
       <c r="C290" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.3">
@@ -27717,7 +27809,7 @@
         <v>306</v>
       </c>
       <c r="C294" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.3">
@@ -27739,7 +27831,7 @@
         <v>308</v>
       </c>
       <c r="C296" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.3">
@@ -27907,10 +27999,10 @@
         <v>67</v>
       </c>
       <c r="C311" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D311" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.3">
@@ -27921,7 +28013,7 @@
         <v>68</v>
       </c>
       <c r="C312" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.3">
@@ -27943,10 +28035,10 @@
         <v>211</v>
       </c>
       <c r="C314" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D314" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.3">
@@ -27957,7 +28049,7 @@
         <v>290</v>
       </c>
       <c r="C315" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.3">
@@ -27968,7 +28060,7 @@
         <v>291</v>
       </c>
       <c r="C316" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.3">
@@ -27979,7 +28071,7 @@
         <v>292</v>
       </c>
       <c r="C317" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.3">
@@ -28023,7 +28115,7 @@
         <v>232</v>
       </c>
       <c r="C321" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.3">
@@ -28034,7 +28126,7 @@
         <v>402</v>
       </c>
       <c r="C322" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.3">
@@ -28056,7 +28148,7 @@
         <v>404</v>
       </c>
       <c r="C324" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.3">
@@ -28067,7 +28159,7 @@
         <v>405</v>
       </c>
       <c r="C325" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.3">
@@ -28078,7 +28170,7 @@
         <v>406</v>
       </c>
       <c r="C326" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.3">
@@ -28089,7 +28181,7 @@
         <v>407</v>
       </c>
       <c r="C327" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.3">
@@ -28100,7 +28192,7 @@
         <v>32</v>
       </c>
       <c r="C328" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.3">
@@ -28111,10 +28203,10 @@
         <v>33</v>
       </c>
       <c r="C329" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D329" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.3">
@@ -28125,7 +28217,7 @@
         <v>213</v>
       </c>
       <c r="C330" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.3">
@@ -28136,7 +28228,7 @@
         <v>267</v>
       </c>
       <c r="C331" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.3">
@@ -28367,7 +28459,7 @@
         <v>203</v>
       </c>
       <c r="C352" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.3">
@@ -28384,7 +28476,7 @@
         <v>570</v>
       </c>
       <c r="E353" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.3">
@@ -28401,7 +28493,7 @@
         <v>570</v>
       </c>
       <c r="E354" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.3">
@@ -28418,7 +28510,7 @@
         <v>570</v>
       </c>
       <c r="E355" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.3">
@@ -28435,7 +28527,7 @@
         <v>570</v>
       </c>
       <c r="E356" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.3">
@@ -28452,7 +28544,7 @@
         <v>570</v>
       </c>
       <c r="E357" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.3">
@@ -28562,7 +28654,7 @@
         <v>94</v>
       </c>
       <c r="C367" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.3">
@@ -28573,7 +28665,7 @@
         <v>95</v>
       </c>
       <c r="C368" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.3">
@@ -28584,7 +28676,7 @@
         <v>96</v>
       </c>
       <c r="C369" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.3">
@@ -28595,7 +28687,7 @@
         <v>97</v>
       </c>
       <c r="C370" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.3">
@@ -28606,7 +28698,7 @@
         <v>98</v>
       </c>
       <c r="C371" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.3">
@@ -28628,7 +28720,7 @@
         <v>314</v>
       </c>
       <c r="C373" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
@@ -28650,7 +28742,7 @@
         <v>63</v>
       </c>
       <c r="C375" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
@@ -28661,7 +28753,7 @@
         <v>64</v>
       </c>
       <c r="C376" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
@@ -28705,7 +28797,7 @@
         <v>283</v>
       </c>
       <c r="C380" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.3">
@@ -28716,7 +28808,7 @@
         <v>284</v>
       </c>
       <c r="C381" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.3">
@@ -28727,7 +28819,7 @@
         <v>285</v>
       </c>
       <c r="C382" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.3">
@@ -28749,7 +28841,7 @@
         <v>441</v>
       </c>
       <c r="C384" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.3">
@@ -28859,7 +28951,7 @@
         <v>227</v>
       </c>
       <c r="C394" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.3">
@@ -28870,7 +28962,7 @@
         <v>228</v>
       </c>
       <c r="C395" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.3">
@@ -28881,7 +28973,7 @@
         <v>229</v>
       </c>
       <c r="C396" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.3">
@@ -28892,7 +28984,7 @@
         <v>230</v>
       </c>
       <c r="C397" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.3">
@@ -28906,7 +28998,7 @@
         <v>546</v>
       </c>
       <c r="D398" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.3">
@@ -28944,7 +29036,7 @@
         <v>287</v>
       </c>
       <c r="C402" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="403" spans="1:8" x14ac:dyDescent="0.3">
@@ -28966,7 +29058,7 @@
         <v>289</v>
       </c>
       <c r="C404" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="405" spans="1:8" x14ac:dyDescent="0.3">
@@ -29254,7 +29346,7 @@
         <v>442</v>
       </c>
       <c r="C431" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.3">
@@ -29265,7 +29357,7 @@
         <v>443</v>
       </c>
       <c r="C432" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.3">
@@ -29276,7 +29368,7 @@
         <v>444</v>
       </c>
       <c r="C433" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.3">
@@ -29472,16 +29564,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -29489,13 +29581,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C2" t="s">
+        <v>808</v>
+      </c>
+      <c r="D2" t="s">
         <v>809</v>
-      </c>
-      <c r="D2" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -29503,10 +29595,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C3" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename readme, improve some comments
</commit_message>
<xml_diff>
--- a/Release/ManiacMansion.xlsx
+++ b/Release/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="14172" windowHeight="7632" tabRatio="702" activeTab="4"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="14172" windowHeight="1872" tabRatio="702" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -3489,8 +3489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4252,7 +4252,7 @@
   <dimension ref="A1:XFD157"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22525,8 +22525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24028,8 +24028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24401,8 +24401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H439"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
+      <selection activeCell="A402" sqref="A402:XFD413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>